<commit_message>
Fixed sheet 3 cases
</commit_message>
<xml_diff>
--- a/utility/TestCases.xlsx
+++ b/utility/TestCases.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FITA_Behave_Proj\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00007DFB-277A-4275-A122-3FD1615039B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CA00CD-4608-4925-8A41-A4980A2CA3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_01" sheetId="1" r:id="rId1"/>
     <sheet name="TC_02" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="TC_03" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
   <si>
     <t>TestCase</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>User click on LoginPage</t>
-  </si>
-  <si>
     <t>TestDescription</t>
   </si>
   <si>
@@ -189,6 +186,39 @@
   </si>
   <si>
     <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>User click on Accordion option from the Widget Tab</t>
+  </si>
+  <si>
+    <t>User click on Practise form option from the Forms Tab</t>
+  </si>
+  <si>
+    <t>User click on TextBox option from the Elements Tab</t>
+  </si>
+  <si>
+    <t>//*[@class="accordion-item"][contains(normalize-space(.), 'What is Lorem Ipsum?')]</t>
+  </si>
+  <si>
+    <t>User click on ''What is Lorem Ipsum?'</t>
+  </si>
+  <si>
+    <t>//*[@class="accordion-item"][contains(normalize-space(.), 'What is Lorem Ipsum?')]//div//p[text()]</t>
+  </si>
+  <si>
+    <t>VerifyText</t>
+  </si>
+  <si>
+    <t>User verifies the description</t>
+  </si>
+  <si>
+    <t>//a[text() = ' Accordion']</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum.</t>
   </si>
 </sst>
 </file>
@@ -545,7 +575,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -561,19 +591,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -587,16 +617,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -608,19 +638,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -631,19 +661,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -654,16 +684,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -674,16 +704,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="4">
         <v>9988776655</v>
@@ -697,16 +727,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="5">
         <v>45915</v>
@@ -720,19 +750,19 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -743,16 +773,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -764,19 +794,19 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -787,19 +817,19 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -810,19 +840,19 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -833,19 +863,19 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -856,16 +886,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -882,13 +912,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE589CD-055B-45D6-ACCC-7E2D19084016}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20.08984375" customWidth="1"/>
     <col min="6" max="6" width="60.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="86.54296875" style="1" bestFit="1" customWidth="1"/>
@@ -899,19 +929,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -919,135 +949,135 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
       <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1061,14 +1091,114 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10529BA-043C-4565-8F99-087106ABCDBF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{3E25D7E7-F9AF-4081-BAE5-7583F4095236}">
+      <formula1>"ElementClick, ClearAndEnter, VerifyText, PrintText, DropdownSelector, Pause"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>